<commit_message>
update rmd and input files
</commit_message>
<xml_diff>
--- a/data/meta.xlsx
+++ b/data/meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nuriteliash/Documents/GitHub/Biological-control-mites-apples/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F4DE35-5660-C143-978E-731B7F81FB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626B60C2-8172-E64C-8752-29546B52B29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12974" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12974" uniqueCount="217">
   <si>
     <t>נזק</t>
   </si>
@@ -686,6 +686,9 @@
   <si>
     <t>22_30</t>
   </si>
+  <si>
+    <t>row</t>
+  </si>
 </sst>
 </file>
 
@@ -22233,7 +22236,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22245,7 +22248,7 @@
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>216</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>32</v>

</xml_diff>